<commit_message>
Double click on List now also accepts entry
</commit_message>
<xml_diff>
--- a/entries.xlsx
+++ b/entries.xlsx
@@ -152,10 +152,10 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.88"/>

</xml_diff>

<commit_message>
Register all entries as people in list and hide ID from list
</commit_message>
<xml_diff>
--- a/entries.xlsx
+++ b/entries.xlsx
@@ -152,10 +152,10 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.88"/>

</xml_diff>

<commit_message>
Using Stack to seperate List view and Form view
</commit_message>
<xml_diff>
--- a/entries.xlsx
+++ b/entries.xlsx
@@ -152,10 +152,10 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.88"/>

</xml_diff>